<commit_message>
update to page layouts/ mew mapping example
</commit_message>
<xml_diff>
--- a/docs/contained-p.xlsx
+++ b/docs/contained-p.xlsx
@@ -1461,9 +1461,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.22265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.203125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
@@ -1471,11 +1471,11 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="102.828125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="96.48828125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="57.05078125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="53.71875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
@@ -1484,22 +1484,22 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="101.46875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.19140625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="95.39453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="47.13671875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="35.3359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="160.9140625" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="41.5625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="24.54296875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.8203125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="151.51171875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="39.390625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="22.9296875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="41.1328125" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="36.43359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add obs profile and extensions
</commit_message>
<xml_diff>
--- a/docs/contained-p.xlsx
+++ b/docs/contained-p.xlsx
@@ -181,7 +181,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id {[]} {[]}
+    <t xml:space="preserve">id
 </t>
   </si>
   <si>
@@ -203,7 +203,7 @@
     <t>Patient.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta {[]} {[]}
+    <t xml:space="preserve">Meta
 </t>
   </si>
   <si>
@@ -219,7 +219,7 @@
     <t>Patient.implicitRules</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -239,7 +239,7 @@
     <t>Patient.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code {[]} {[]}
+    <t xml:space="preserve">code
 </t>
   </si>
   <si>
@@ -271,7 +271,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative {[]} {[]}
+    <t xml:space="preserve">Narrative
 </t>
   </si>
   <si>
@@ -301,7 +301,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource {[]} {[]}
+    <t xml:space="preserve">Resource
 </t>
   </si>
   <si>
@@ -327,7 +327,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
@@ -358,7 +358,7 @@
     <t>Patient.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier {[]} {[]}
+    <t xml:space="preserve">Identifier
 </t>
   </si>
   <si>
@@ -383,7 +383,7 @@
     <t>Patient.identifier.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -451,7 +451,7 @@
     <t>Patient.identifier.type</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
+    <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
@@ -495,7 +495,7 @@
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.acme.com/identifiers/patient or urn:ietf:rfc:3986 if the Identifier.value itself is a full uri"/&gt;</t>
+    <t>http://www.acme.com/identifiers/patient or urn:ietf:rfc:3986 if the Identifier.value itself is a full uri</t>
   </si>
   <si>
     <t>Identifier.system</t>
@@ -519,7 +519,7 @@
     <t>The actual patient identifier value.</t>
   </si>
   <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="123456"/&gt;</t>
+    <t>123456</t>
   </si>
   <si>
     <t>Identifier.value</t>
@@ -534,7 +534,7 @@
     <t>Patient.identifier.period</t>
   </si>
   <si>
-    <t xml:space="preserve">Period {[]} {[]}
+    <t xml:space="preserve">Period
 </t>
   </si>
   <si>
@@ -556,7 +556,7 @@
     <t>Patient.identifier.assigner</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
+    <t xml:space="preserve">Reference(Organization)
 </t>
   </si>
   <si>
@@ -581,7 +581,7 @@
     <t>Patient.active</t>
   </si>
   <si>
-    <t xml:space="preserve">boolean {[]} {[]}
+    <t xml:space="preserve">boolean
 </t>
   </si>
   <si>
@@ -598,7 +598,7 @@
     <t>Need to be able to mark a patient record as not to be used because it was created in error.</t>
   </si>
   <si>
-    <t>&lt;valueBoolean xmlns="http://hl7.org/fhir" value="true"/&gt;</t>
+    <t>true</t>
   </si>
   <si>
     <t>statusCode</t>
@@ -610,7 +610,7 @@
     <t>Patient.name</t>
   </si>
   <si>
-    <t xml:space="preserve">HumanName {[]} {[]}
+    <t xml:space="preserve">HumanName
 </t>
   </si>
   <si>
@@ -638,7 +638,7 @@
     <t>Patient.telecom</t>
   </si>
   <si>
-    <t xml:space="preserve">ContactPoint {[]} {[]}
+    <t xml:space="preserve">ContactPoint
 </t>
   </si>
   <si>
@@ -696,7 +696,7 @@
     <t>Patient.birthDate</t>
   </si>
   <si>
-    <t xml:space="preserve">date {[]} {[]}
+    <t xml:space="preserve">date
 </t>
   </si>
   <si>
@@ -727,8 +727,8 @@
     <t>Patient.deceased[x]</t>
   </si>
   <si>
-    <t>boolean {[]} {[]}
-dateTime {[]} {[]}</t>
+    <t>boolean
+dateTime</t>
   </si>
   <si>
     <t>Indicates if the individual is deceased or not</t>
@@ -753,7 +753,7 @@
     <t>Patient.address</t>
   </si>
   <si>
-    <t xml:space="preserve">Address {[]} {[]}
+    <t xml:space="preserve">Address
 </t>
   </si>
   <si>
@@ -808,8 +808,8 @@
     <t>Patient.multipleBirth[x]</t>
   </si>
   <si>
-    <t>boolean {[]} {[]}
-integer {[]} {[]}</t>
+    <t>boolean
+integer</t>
   </si>
   <si>
     <t>Whether patient is part of a multiple birth</t>
@@ -835,7 +835,7 @@
     <t>Patient.photo</t>
   </si>
   <si>
-    <t xml:space="preserve">Attachment {[]} {[]}
+    <t xml:space="preserve">Attachment
 </t>
   </si>
   <si>
@@ -857,7 +857,7 @@
     <t>Patient.contact</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement {[]} {[]}
+    <t xml:space="preserve">BackboneElement
 </t>
   </si>
   <si>
@@ -1205,7 +1205,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization], CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner]]}
+    <t xml:space="preserve">Reference(Organization|Practitioner)
 </t>
   </si>
   <si>
@@ -1275,7 +1275,7 @@
     <t>Patient.link.other</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
+    <t xml:space="preserve">Reference(Patient|RelatedPerson)
 </t>
   </si>
   <si>
@@ -1356,67 +1356,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -1452,7 +1452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO61"/>
+  <dimension ref="A1:AN61"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1475,7 +1475,7 @@
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="53.71875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>

</xml_diff>